<commit_message>
Excel Import Material Receipt Stock Entry : thay thay đổi thứ tự cột
</commit_message>
<xml_diff>
--- a/customize_erpnext/api/bulk_update_scripts/create_material_issue_teamplate.xlsx
+++ b/customize_erpnext/api/bulk_update_scripts/create_material_issue_teamplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\son.nt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9918F6C1-5CE1-4ED3-AFFC-BFE3E33FF879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8091EE-B4EA-44F7-A49B-FCE69F0F3F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D1FB37B-ACCB-49B7-B149-95779F24E43C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6D1FB37B-ACCB-49B7-B149-95779F24E43C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -1320,26 +1320,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -1364,6 +1344,26 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1681,25 +1681,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23D4B30C-D8CA-4512-B19C-3C1EA571E46D}" name="Table2" displayName="Table2" ref="A1:Q197" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23D4B30C-D8CA-4512-B19C-3C1EA571E46D}" name="Table2" displayName="Table2" ref="A1:Q197" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:Q197" xr:uid="{23D4B30C-D8CA-4512-B19C-3C1EA571E46D}"/>
   <tableColumns count="17">
     <tableColumn id="4" xr3:uid="{43B4B1C8-2F98-4655-B691-168EDDCCE375}" name="Index"/>
     <tableColumn id="5" xr3:uid="{E368165F-11C4-4A20-8BD2-79B3767B3339}" name="stock_entry_type"/>
-    <tableColumn id="1" xr3:uid="{AC16C6E8-21F8-4CEF-AECE-A640C10BF15C}" name="posting_date" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{DF8DC880-8EBD-4FE7-9E87-36E78396FC1D}" name="posting_time" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{AC16C6E8-21F8-4CEF-AECE-A640C10BF15C}" name="posting_date" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{DF8DC880-8EBD-4FE7-9E87-36E78396FC1D}" name="posting_time" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{1C2EE34F-C702-4828-AA4B-D9BFB98CAD12}" name="custom_no"/>
     <tableColumn id="3" xr3:uid="{B681AA7B-0BC4-4606-BA37-476C0A4AF900}" name="custom_material_issue_purpose"/>
+    <tableColumn id="7" xr3:uid="{49AC4B6D-D4F4-45DA-AFD8-B6F8C84E00BD}" name="custom_fg_style"/>
     <tableColumn id="8" xr3:uid="{A0270107-0F84-476C-B8BF-87B64620A48F}" name="custom_fg_size"/>
-    <tableColumn id="7" xr3:uid="{49AC4B6D-D4F4-45DA-AFD8-B6F8C84E00BD}" name="custom_fg_style"/>
     <tableColumn id="9" xr3:uid="{395CAF36-02BF-4FF2-A938-B6C6AAEF0F08}" name="custom_fg_qty"/>
     <tableColumn id="10" xr3:uid="{6A6222F5-7986-4D51-BBF1-416706649393}" name="custom_line"/>
     <tableColumn id="11" xr3:uid="{A4722DCB-058E-41BE-984B-8C716DCA28EC}" name="custom_fg_color"/>
     <tableColumn id="12" xr3:uid="{4893C9B7-1C3A-4701-9A29-8196008DB078}" name="custom_note"/>
     <tableColumn id="16" xr3:uid="{716EBAAA-6185-464A-9B5C-6EEEEF9710A1}" name="item_code"/>
     <tableColumn id="14" xr3:uid="{81D9E945-17C9-4C18-B369-64BDB74B641C}" name="custom_item_name_detail"/>
-    <tableColumn id="6" xr3:uid="{FC72D5FE-5469-4162-9475-201BDE3D3996}" name="qty" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{A168D37F-FF1F-4C20-92EC-5863804C308C}" name="s_warehouse" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{FC72D5FE-5469-4162-9475-201BDE3D3996}" name="qty" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{A168D37F-FF1F-4C20-92EC-5863804C308C}" name="s_warehouse" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{77F6BB6F-831A-4EF5-B17F-D18C79F5E860}" name="custom_invoice_number"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2026,7 +2026,7 @@
   <dimension ref="A1:Q197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,16 +2034,19 @@
     <col min="3" max="4" width="14.21875" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
-    <col min="15" max="16" width="17.21875" customWidth="1"/>
-    <col min="17" max="17" width="24.33203125" customWidth="1"/>
-    <col min="18" max="19" width="14.33203125" customWidth="1"/>
-    <col min="20" max="20" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="10" max="10" width="23.77734375" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" customWidth="1"/>
+    <col min="14" max="14" width="16.5546875" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="17" width="17.21875" customWidth="1"/>
+    <col min="18" max="18" width="24.33203125" customWidth="1"/>
+    <col min="19" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="21" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -2066,10 +2069,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>12</v>
@@ -2119,10 +2122,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>370</v>
+      </c>
+      <c r="H2" t="s">
         <v>210</v>
-      </c>
-      <c r="H2" t="s">
-        <v>370</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
@@ -2169,10 +2172,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
+        <v>370</v>
+      </c>
+      <c r="H3" t="s">
         <v>210</v>
-      </c>
-      <c r="H3" t="s">
-        <v>370</v>
       </c>
       <c r="J3" t="s">
         <v>0</v>
@@ -2219,10 +2222,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
+        <v>370</v>
+      </c>
+      <c r="H4" t="s">
         <v>210</v>
-      </c>
-      <c r="H4" t="s">
-        <v>370</v>
       </c>
       <c r="J4" t="s">
         <v>1</v>
@@ -2269,10 +2272,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
+        <v>370</v>
+      </c>
+      <c r="H5" t="s">
         <v>210</v>
-      </c>
-      <c r="H5" t="s">
-        <v>370</v>
       </c>
       <c r="J5" t="s">
         <v>1</v>
@@ -2319,10 +2322,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
+        <v>370</v>
+      </c>
+      <c r="H6" t="s">
         <v>210</v>
-      </c>
-      <c r="H6" t="s">
-        <v>370</v>
       </c>
       <c r="J6" t="s">
         <v>0</v>
@@ -2369,10 +2372,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
+        <v>370</v>
+      </c>
+      <c r="H7" t="s">
         <v>210</v>
-      </c>
-      <c r="H7" t="s">
-        <v>370</v>
       </c>
       <c r="J7" t="s">
         <v>0</v>
@@ -2419,10 +2422,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
+        <v>370</v>
+      </c>
+      <c r="H8" t="s">
         <v>210</v>
-      </c>
-      <c r="H8" t="s">
-        <v>370</v>
       </c>
       <c r="J8" t="s">
         <v>0</v>
@@ -2469,10 +2472,10 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
+        <v>371</v>
+      </c>
+      <c r="H9" t="s">
         <v>210</v>
-      </c>
-      <c r="H9" t="s">
-        <v>371</v>
       </c>
       <c r="I9">
         <v>201</v>
@@ -2522,10 +2525,10 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
+        <v>371</v>
+      </c>
+      <c r="H10" t="s">
         <v>210</v>
-      </c>
-      <c r="H10" t="s">
-        <v>371</v>
       </c>
       <c r="I10">
         <v>201</v>
@@ -2575,10 +2578,10 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
+        <v>371</v>
+      </c>
+      <c r="H11" t="s">
         <v>210</v>
-      </c>
-      <c r="H11" t="s">
-        <v>371</v>
       </c>
       <c r="I11">
         <v>201</v>
@@ -2628,10 +2631,10 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
+        <v>371</v>
+      </c>
+      <c r="H12" t="s">
         <v>210</v>
-      </c>
-      <c r="H12" t="s">
-        <v>371</v>
       </c>
       <c r="I12">
         <v>201</v>
@@ -2681,10 +2684,10 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
+        <v>371</v>
+      </c>
+      <c r="H13" t="s">
         <v>210</v>
-      </c>
-      <c r="H13" t="s">
-        <v>371</v>
       </c>
       <c r="I13">
         <v>201</v>
@@ -2734,10 +2737,10 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
+        <v>371</v>
+      </c>
+      <c r="H14" t="s">
         <v>210</v>
-      </c>
-      <c r="H14" t="s">
-        <v>371</v>
       </c>
       <c r="I14">
         <v>201</v>
@@ -2787,10 +2790,10 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
+        <v>371</v>
+      </c>
+      <c r="H15" t="s">
         <v>210</v>
-      </c>
-      <c r="H15" t="s">
-        <v>371</v>
       </c>
       <c r="I15">
         <v>201</v>
@@ -2840,10 +2843,10 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
+        <v>371</v>
+      </c>
+      <c r="H16" t="s">
         <v>210</v>
-      </c>
-      <c r="H16" t="s">
-        <v>371</v>
       </c>
       <c r="I16">
         <v>201</v>
@@ -2893,10 +2896,10 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
+        <v>371</v>
+      </c>
+      <c r="H17" t="s">
         <v>210</v>
-      </c>
-      <c r="H17" t="s">
-        <v>371</v>
       </c>
       <c r="I17">
         <v>201</v>
@@ -2946,10 +2949,10 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
+        <v>371</v>
+      </c>
+      <c r="H18" t="s">
         <v>210</v>
-      </c>
-      <c r="H18" t="s">
-        <v>371</v>
       </c>
       <c r="I18">
         <v>201</v>
@@ -2999,10 +3002,10 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
+        <v>371</v>
+      </c>
+      <c r="H19" t="s">
         <v>210</v>
-      </c>
-      <c r="H19" t="s">
-        <v>371</v>
       </c>
       <c r="I19">
         <v>201</v>
@@ -3052,10 +3055,10 @@
         <v>2</v>
       </c>
       <c r="G20" t="s">
+        <v>371</v>
+      </c>
+      <c r="H20" t="s">
         <v>210</v>
-      </c>
-      <c r="H20" t="s">
-        <v>371</v>
       </c>
       <c r="I20">
         <v>201</v>
@@ -3105,10 +3108,10 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
+        <v>371</v>
+      </c>
+      <c r="H21" t="s">
         <v>210</v>
-      </c>
-      <c r="H21" t="s">
-        <v>371</v>
       </c>
       <c r="I21">
         <v>201</v>
@@ -3158,10 +3161,10 @@
         <v>2</v>
       </c>
       <c r="G22" t="s">
+        <v>371</v>
+      </c>
+      <c r="H22" t="s">
         <v>210</v>
-      </c>
-      <c r="H22" t="s">
-        <v>371</v>
       </c>
       <c r="I22">
         <v>201</v>
@@ -3211,10 +3214,10 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H23" t="s">
         <v>210</v>
-      </c>
-      <c r="H23" t="s">
-        <v>371</v>
       </c>
       <c r="I23">
         <v>201</v>
@@ -3264,10 +3267,10 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
+        <v>371</v>
+      </c>
+      <c r="H24" t="s">
         <v>210</v>
-      </c>
-      <c r="H24" t="s">
-        <v>371</v>
       </c>
       <c r="I24">
         <v>201</v>
@@ -3317,10 +3320,10 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
+        <v>371</v>
+      </c>
+      <c r="H25" t="s">
         <v>210</v>
-      </c>
-      <c r="H25" t="s">
-        <v>371</v>
       </c>
       <c r="I25">
         <v>201</v>
@@ -3370,10 +3373,10 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
+        <v>371</v>
+      </c>
+      <c r="H26" t="s">
         <v>210</v>
-      </c>
-      <c r="H26" t="s">
-        <v>371</v>
       </c>
       <c r="I26">
         <v>201</v>
@@ -3423,10 +3426,10 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
+        <v>371</v>
+      </c>
+      <c r="H27" t="s">
         <v>210</v>
-      </c>
-      <c r="H27" t="s">
-        <v>371</v>
       </c>
       <c r="I27">
         <v>201</v>
@@ -3476,10 +3479,10 @@
         <v>2</v>
       </c>
       <c r="G28" t="s">
+        <v>371</v>
+      </c>
+      <c r="H28" t="s">
         <v>210</v>
-      </c>
-      <c r="H28" t="s">
-        <v>371</v>
       </c>
       <c r="I28">
         <v>201</v>
@@ -3529,10 +3532,10 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
+        <v>371</v>
+      </c>
+      <c r="H29" t="s">
         <v>210</v>
-      </c>
-      <c r="H29" t="s">
-        <v>371</v>
       </c>
       <c r="I29">
         <v>201</v>
@@ -3582,10 +3585,10 @@
         <v>2</v>
       </c>
       <c r="G30" t="s">
+        <v>371</v>
+      </c>
+      <c r="H30" t="s">
         <v>210</v>
-      </c>
-      <c r="H30" t="s">
-        <v>371</v>
       </c>
       <c r="I30">
         <v>201</v>
@@ -3635,10 +3638,10 @@
         <v>2</v>
       </c>
       <c r="G31" t="s">
+        <v>371</v>
+      </c>
+      <c r="H31" t="s">
         <v>210</v>
-      </c>
-      <c r="H31" t="s">
-        <v>371</v>
       </c>
       <c r="I31">
         <v>201</v>
@@ -3688,10 +3691,10 @@
         <v>2</v>
       </c>
       <c r="G32" t="s">
+        <v>371</v>
+      </c>
+      <c r="H32" t="s">
         <v>210</v>
-      </c>
-      <c r="H32" t="s">
-        <v>371</v>
       </c>
       <c r="I32">
         <v>201</v>
@@ -3741,10 +3744,10 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
+        <v>371</v>
+      </c>
+      <c r="H33" t="s">
         <v>210</v>
-      </c>
-      <c r="H33" t="s">
-        <v>371</v>
       </c>
       <c r="I33">
         <v>266</v>
@@ -3794,10 +3797,10 @@
         <v>2</v>
       </c>
       <c r="G34" t="s">
+        <v>371</v>
+      </c>
+      <c r="H34" t="s">
         <v>210</v>
-      </c>
-      <c r="H34" t="s">
-        <v>371</v>
       </c>
       <c r="I34">
         <v>266</v>
@@ -3847,10 +3850,10 @@
         <v>2</v>
       </c>
       <c r="G35" t="s">
+        <v>371</v>
+      </c>
+      <c r="H35" t="s">
         <v>210</v>
-      </c>
-      <c r="H35" t="s">
-        <v>371</v>
       </c>
       <c r="I35">
         <v>266</v>
@@ -3900,10 +3903,10 @@
         <v>2</v>
       </c>
       <c r="G36" t="s">
+        <v>371</v>
+      </c>
+      <c r="H36" t="s">
         <v>210</v>
-      </c>
-      <c r="H36" t="s">
-        <v>371</v>
       </c>
       <c r="I36">
         <v>266</v>
@@ -3953,10 +3956,10 @@
         <v>2</v>
       </c>
       <c r="G37" t="s">
+        <v>371</v>
+      </c>
+      <c r="H37" t="s">
         <v>210</v>
-      </c>
-      <c r="H37" t="s">
-        <v>371</v>
       </c>
       <c r="I37">
         <v>266</v>
@@ -4006,10 +4009,10 @@
         <v>2</v>
       </c>
       <c r="G38" t="s">
+        <v>371</v>
+      </c>
+      <c r="H38" t="s">
         <v>210</v>
-      </c>
-      <c r="H38" t="s">
-        <v>371</v>
       </c>
       <c r="I38">
         <v>266</v>
@@ -4059,10 +4062,10 @@
         <v>2</v>
       </c>
       <c r="G39" t="s">
+        <v>371</v>
+      </c>
+      <c r="H39" t="s">
         <v>210</v>
-      </c>
-      <c r="H39" t="s">
-        <v>371</v>
       </c>
       <c r="I39">
         <v>266</v>
@@ -4112,10 +4115,10 @@
         <v>2</v>
       </c>
       <c r="G40" t="s">
+        <v>371</v>
+      </c>
+      <c r="H40" t="s">
         <v>210</v>
-      </c>
-      <c r="H40" t="s">
-        <v>371</v>
       </c>
       <c r="I40">
         <v>266</v>
@@ -4165,10 +4168,10 @@
         <v>2</v>
       </c>
       <c r="G41" t="s">
+        <v>371</v>
+      </c>
+      <c r="H41" t="s">
         <v>210</v>
-      </c>
-      <c r="H41" t="s">
-        <v>371</v>
       </c>
       <c r="I41">
         <v>266</v>
@@ -4218,10 +4221,10 @@
         <v>2</v>
       </c>
       <c r="G42" t="s">
+        <v>371</v>
+      </c>
+      <c r="H42" t="s">
         <v>210</v>
-      </c>
-      <c r="H42" t="s">
-        <v>371</v>
       </c>
       <c r="I42">
         <v>266</v>
@@ -4271,10 +4274,10 @@
         <v>2</v>
       </c>
       <c r="G43" t="s">
+        <v>371</v>
+      </c>
+      <c r="H43" t="s">
         <v>210</v>
-      </c>
-      <c r="H43" t="s">
-        <v>371</v>
       </c>
       <c r="I43">
         <v>266</v>
@@ -4324,10 +4327,10 @@
         <v>2</v>
       </c>
       <c r="G44" t="s">
+        <v>371</v>
+      </c>
+      <c r="H44" t="s">
         <v>210</v>
-      </c>
-      <c r="H44" t="s">
-        <v>371</v>
       </c>
       <c r="I44">
         <v>266</v>
@@ -4377,10 +4380,10 @@
         <v>2</v>
       </c>
       <c r="G45" t="s">
+        <v>371</v>
+      </c>
+      <c r="H45" t="s">
         <v>210</v>
-      </c>
-      <c r="H45" t="s">
-        <v>371</v>
       </c>
       <c r="I45">
         <v>266</v>
@@ -4430,10 +4433,10 @@
         <v>2</v>
       </c>
       <c r="G46" t="s">
+        <v>371</v>
+      </c>
+      <c r="H46" t="s">
         <v>210</v>
-      </c>
-      <c r="H46" t="s">
-        <v>371</v>
       </c>
       <c r="I46">
         <v>266</v>
@@ -4483,10 +4486,10 @@
         <v>2</v>
       </c>
       <c r="G47" t="s">
+        <v>371</v>
+      </c>
+      <c r="H47" t="s">
         <v>210</v>
-      </c>
-      <c r="H47" t="s">
-        <v>371</v>
       </c>
       <c r="I47">
         <v>266</v>
@@ -4536,10 +4539,10 @@
         <v>2</v>
       </c>
       <c r="G48" t="s">
+        <v>371</v>
+      </c>
+      <c r="H48" t="s">
         <v>210</v>
-      </c>
-      <c r="H48" t="s">
-        <v>371</v>
       </c>
       <c r="I48">
         <v>266</v>
@@ -4589,10 +4592,10 @@
         <v>2</v>
       </c>
       <c r="G49" t="s">
+        <v>371</v>
+      </c>
+      <c r="H49" t="s">
         <v>210</v>
-      </c>
-      <c r="H49" t="s">
-        <v>371</v>
       </c>
       <c r="I49">
         <v>266</v>
@@ -4642,10 +4645,10 @@
         <v>2</v>
       </c>
       <c r="G50" t="s">
+        <v>371</v>
+      </c>
+      <c r="H50" t="s">
         <v>210</v>
-      </c>
-      <c r="H50" t="s">
-        <v>371</v>
       </c>
       <c r="I50">
         <v>266</v>
@@ -4695,10 +4698,10 @@
         <v>2</v>
       </c>
       <c r="G51" t="s">
+        <v>371</v>
+      </c>
+      <c r="H51" t="s">
         <v>210</v>
-      </c>
-      <c r="H51" t="s">
-        <v>371</v>
       </c>
       <c r="I51">
         <v>266</v>
@@ -4748,10 +4751,10 @@
         <v>2</v>
       </c>
       <c r="G52" t="s">
+        <v>371</v>
+      </c>
+      <c r="H52" t="s">
         <v>210</v>
-      </c>
-      <c r="H52" t="s">
-        <v>371</v>
       </c>
       <c r="I52">
         <v>266</v>
@@ -4801,10 +4804,10 @@
         <v>2</v>
       </c>
       <c r="G53" t="s">
+        <v>371</v>
+      </c>
+      <c r="H53" t="s">
         <v>210</v>
-      </c>
-      <c r="H53" t="s">
-        <v>371</v>
       </c>
       <c r="I53">
         <v>266</v>
@@ -4854,10 +4857,10 @@
         <v>2</v>
       </c>
       <c r="G54" t="s">
+        <v>371</v>
+      </c>
+      <c r="H54" t="s">
         <v>210</v>
-      </c>
-      <c r="H54" t="s">
-        <v>371</v>
       </c>
       <c r="I54">
         <v>266</v>
@@ -4907,10 +4910,10 @@
         <v>2</v>
       </c>
       <c r="G55" t="s">
+        <v>371</v>
+      </c>
+      <c r="H55" t="s">
         <v>210</v>
-      </c>
-      <c r="H55" t="s">
-        <v>371</v>
       </c>
       <c r="I55">
         <v>266</v>
@@ -4960,10 +4963,10 @@
         <v>2</v>
       </c>
       <c r="G56" t="s">
+        <v>371</v>
+      </c>
+      <c r="H56" t="s">
         <v>210</v>
-      </c>
-      <c r="H56" t="s">
-        <v>371</v>
       </c>
       <c r="I56">
         <v>266</v>
@@ -5013,10 +5016,10 @@
         <v>2</v>
       </c>
       <c r="G57" t="s">
+        <v>371</v>
+      </c>
+      <c r="H57" t="s">
         <v>210</v>
-      </c>
-      <c r="H57" t="s">
-        <v>371</v>
       </c>
       <c r="I57">
         <v>266</v>
@@ -5066,10 +5069,10 @@
         <v>2</v>
       </c>
       <c r="G58" t="s">
+        <v>371</v>
+      </c>
+      <c r="H58" t="s">
         <v>210</v>
-      </c>
-      <c r="H58" t="s">
-        <v>371</v>
       </c>
       <c r="I58">
         <v>266</v>
@@ -5119,10 +5122,10 @@
         <v>2</v>
       </c>
       <c r="G59" t="s">
+        <v>371</v>
+      </c>
+      <c r="H59" t="s">
         <v>210</v>
-      </c>
-      <c r="H59" t="s">
-        <v>371</v>
       </c>
       <c r="I59">
         <v>266</v>
@@ -5172,10 +5175,10 @@
         <v>2</v>
       </c>
       <c r="G60" t="s">
+        <v>371</v>
+      </c>
+      <c r="H60" t="s">
         <v>210</v>
-      </c>
-      <c r="H60" t="s">
-        <v>371</v>
       </c>
       <c r="I60">
         <v>266</v>
@@ -5225,10 +5228,10 @@
         <v>2</v>
       </c>
       <c r="G61" t="s">
+        <v>371</v>
+      </c>
+      <c r="H61" t="s">
         <v>210</v>
-      </c>
-      <c r="H61" t="s">
-        <v>371</v>
       </c>
       <c r="I61">
         <v>266</v>
@@ -5278,10 +5281,10 @@
         <v>2</v>
       </c>
       <c r="G62" t="s">
+        <v>371</v>
+      </c>
+      <c r="H62" t="s">
         <v>210</v>
-      </c>
-      <c r="H62" t="s">
-        <v>371</v>
       </c>
       <c r="I62">
         <v>266</v>
@@ -5331,10 +5334,10 @@
         <v>2</v>
       </c>
       <c r="G63" t="s">
+        <v>372</v>
+      </c>
+      <c r="H63" t="s">
         <v>210</v>
-      </c>
-      <c r="H63" t="s">
-        <v>372</v>
       </c>
       <c r="I63">
         <v>314</v>
@@ -5384,10 +5387,10 @@
         <v>2</v>
       </c>
       <c r="G64" t="s">
+        <v>372</v>
+      </c>
+      <c r="H64" t="s">
         <v>210</v>
-      </c>
-      <c r="H64" t="s">
-        <v>372</v>
       </c>
       <c r="I64">
         <v>314</v>
@@ -5437,10 +5440,10 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
+        <v>372</v>
+      </c>
+      <c r="H65" t="s">
         <v>210</v>
-      </c>
-      <c r="H65" t="s">
-        <v>372</v>
       </c>
       <c r="I65">
         <v>314</v>
@@ -5490,10 +5493,10 @@
         <v>2</v>
       </c>
       <c r="G66" t="s">
+        <v>372</v>
+      </c>
+      <c r="H66" t="s">
         <v>210</v>
-      </c>
-      <c r="H66" t="s">
-        <v>372</v>
       </c>
       <c r="I66">
         <v>314</v>
@@ -5543,10 +5546,10 @@
         <v>2</v>
       </c>
       <c r="G67" t="s">
+        <v>372</v>
+      </c>
+      <c r="H67" t="s">
         <v>210</v>
-      </c>
-      <c r="H67" t="s">
-        <v>372</v>
       </c>
       <c r="I67">
         <v>314</v>
@@ -5596,10 +5599,10 @@
         <v>2</v>
       </c>
       <c r="G68" t="s">
+        <v>372</v>
+      </c>
+      <c r="H68" t="s">
         <v>210</v>
-      </c>
-      <c r="H68" t="s">
-        <v>372</v>
       </c>
       <c r="I68">
         <v>314</v>
@@ -5649,10 +5652,10 @@
         <v>2</v>
       </c>
       <c r="G69" t="s">
+        <v>372</v>
+      </c>
+      <c r="H69" t="s">
         <v>210</v>
-      </c>
-      <c r="H69" t="s">
-        <v>372</v>
       </c>
       <c r="I69">
         <v>314</v>
@@ -5702,10 +5705,10 @@
         <v>2</v>
       </c>
       <c r="G70" t="s">
+        <v>372</v>
+      </c>
+      <c r="H70" t="s">
         <v>210</v>
-      </c>
-      <c r="H70" t="s">
-        <v>372</v>
       </c>
       <c r="I70">
         <v>314</v>
@@ -5755,10 +5758,10 @@
         <v>2</v>
       </c>
       <c r="G71" t="s">
+        <v>372</v>
+      </c>
+      <c r="H71" t="s">
         <v>210</v>
-      </c>
-      <c r="H71" t="s">
-        <v>372</v>
       </c>
       <c r="I71">
         <v>314</v>
@@ -5808,10 +5811,10 @@
         <v>2</v>
       </c>
       <c r="G72" t="s">
+        <v>372</v>
+      </c>
+      <c r="H72" t="s">
         <v>210</v>
-      </c>
-      <c r="H72" t="s">
-        <v>372</v>
       </c>
       <c r="I72">
         <v>314</v>
@@ -9097,7 +9100,7 @@
       <c r="E145" t="s">
         <v>41</v>
       </c>
-      <c r="G145" t="s">
+      <c r="H145" t="s">
         <v>1</v>
       </c>
       <c r="I145" t="s">
@@ -9139,7 +9142,7 @@
       <c r="E146" t="s">
         <v>41</v>
       </c>
-      <c r="G146" t="s">
+      <c r="H146" t="s">
         <v>1</v>
       </c>
       <c r="I146" t="s">
@@ -9181,7 +9184,7 @@
       <c r="E147" t="s">
         <v>41</v>
       </c>
-      <c r="G147" t="s">
+      <c r="H147" t="s">
         <v>1</v>
       </c>
       <c r="I147" t="s">
@@ -9223,7 +9226,7 @@
       <c r="E148" t="s">
         <v>41</v>
       </c>
-      <c r="G148" t="s">
+      <c r="H148" t="s">
         <v>1</v>
       </c>
       <c r="I148" t="s">
@@ -9265,7 +9268,7 @@
       <c r="E149" t="s">
         <v>41</v>
       </c>
-      <c r="G149" t="s">
+      <c r="H149" t="s">
         <v>1</v>
       </c>
       <c r="I149" t="s">
@@ -9307,7 +9310,7 @@
       <c r="E150" t="s">
         <v>41</v>
       </c>
-      <c r="G150" t="s">
+      <c r="H150" t="s">
         <v>1</v>
       </c>
       <c r="I150" t="s">
@@ -9349,7 +9352,7 @@
       <c r="E151" t="s">
         <v>41</v>
       </c>
-      <c r="G151" t="s">
+      <c r="H151" t="s">
         <v>1</v>
       </c>
       <c r="I151" t="s">
@@ -9391,7 +9394,7 @@
       <c r="E152" t="s">
         <v>41</v>
       </c>
-      <c r="G152" t="s">
+      <c r="H152" t="s">
         <v>1</v>
       </c>
       <c r="I152" t="s">
@@ -9433,7 +9436,7 @@
       <c r="E153" t="s">
         <v>41</v>
       </c>
-      <c r="G153" t="s">
+      <c r="H153" t="s">
         <v>1</v>
       </c>
       <c r="I153" t="s">
@@ -9475,7 +9478,7 @@
       <c r="E154" t="s">
         <v>41</v>
       </c>
-      <c r="G154" t="s">
+      <c r="H154" t="s">
         <v>1</v>
       </c>
       <c r="I154" t="s">
@@ -9517,7 +9520,7 @@
       <c r="E155" t="s">
         <v>41</v>
       </c>
-      <c r="G155" t="s">
+      <c r="H155" t="s">
         <v>1</v>
       </c>
       <c r="I155" t="s">
@@ -9559,7 +9562,7 @@
       <c r="E156" t="s">
         <v>41</v>
       </c>
-      <c r="G156" t="s">
+      <c r="H156" t="s">
         <v>1</v>
       </c>
       <c r="I156" t="s">
@@ -9601,7 +9604,7 @@
       <c r="E157" t="s">
         <v>41</v>
       </c>
-      <c r="G157" t="s">
+      <c r="H157" t="s">
         <v>1</v>
       </c>
       <c r="I157" t="s">
@@ -9643,7 +9646,7 @@
       <c r="E158" t="s">
         <v>41</v>
       </c>
-      <c r="G158" t="s">
+      <c r="H158" t="s">
         <v>1</v>
       </c>
       <c r="I158" t="s">
@@ -9685,7 +9688,7 @@
       <c r="E159" t="s">
         <v>41</v>
       </c>
-      <c r="G159" t="s">
+      <c r="H159" t="s">
         <v>1</v>
       </c>
       <c r="I159" t="s">
@@ -9727,7 +9730,7 @@
       <c r="E160" t="s">
         <v>41</v>
       </c>
-      <c r="G160" t="s">
+      <c r="H160" t="s">
         <v>1</v>
       </c>
       <c r="I160" t="s">
@@ -9769,7 +9772,7 @@
       <c r="E161" t="s">
         <v>41</v>
       </c>
-      <c r="G161" t="s">
+      <c r="H161" t="s">
         <v>1</v>
       </c>
       <c r="I161" t="s">
@@ -9811,7 +9814,7 @@
       <c r="E162" t="s">
         <v>41</v>
       </c>
-      <c r="G162" t="s">
+      <c r="H162" t="s">
         <v>1</v>
       </c>
       <c r="I162" t="s">
@@ -9853,7 +9856,7 @@
       <c r="E163" t="s">
         <v>41</v>
       </c>
-      <c r="G163" t="s">
+      <c r="H163" t="s">
         <v>1</v>
       </c>
       <c r="I163" t="s">
@@ -9895,7 +9898,7 @@
       <c r="E164" t="s">
         <v>41</v>
       </c>
-      <c r="G164" t="s">
+      <c r="H164" t="s">
         <v>1</v>
       </c>
       <c r="I164" t="s">
@@ -9937,7 +9940,7 @@
       <c r="E165" t="s">
         <v>41</v>
       </c>
-      <c r="G165" t="s">
+      <c r="H165" t="s">
         <v>1</v>
       </c>
       <c r="I165" t="s">
@@ -9979,7 +9982,7 @@
       <c r="E166" t="s">
         <v>41</v>
       </c>
-      <c r="G166" t="s">
+      <c r="H166" t="s">
         <v>1</v>
       </c>
       <c r="I166" t="s">
@@ -10021,7 +10024,7 @@
       <c r="E167" t="s">
         <v>41</v>
       </c>
-      <c r="G167" t="s">
+      <c r="H167" t="s">
         <v>1</v>
       </c>
       <c r="I167" t="s">
@@ -10063,7 +10066,7 @@
       <c r="E168" t="s">
         <v>41</v>
       </c>
-      <c r="G168" t="s">
+      <c r="H168" t="s">
         <v>1</v>
       </c>
       <c r="I168" t="s">
@@ -10105,7 +10108,7 @@
       <c r="E169" t="s">
         <v>41</v>
       </c>
-      <c r="G169" t="s">
+      <c r="H169" t="s">
         <v>1</v>
       </c>
       <c r="I169" t="s">
@@ -10147,7 +10150,7 @@
       <c r="E170" t="s">
         <v>41</v>
       </c>
-      <c r="G170" t="s">
+      <c r="H170" t="s">
         <v>1</v>
       </c>
       <c r="I170" t="s">
@@ -10189,7 +10192,7 @@
       <c r="E171" t="s">
         <v>41</v>
       </c>
-      <c r="G171" t="s">
+      <c r="H171" t="s">
         <v>1</v>
       </c>
       <c r="I171" t="s">
@@ -10231,7 +10234,7 @@
       <c r="E172" t="s">
         <v>41</v>
       </c>
-      <c r="G172" t="s">
+      <c r="H172" t="s">
         <v>1</v>
       </c>
       <c r="I172" t="s">
@@ -10273,7 +10276,7 @@
       <c r="E173" t="s">
         <v>41</v>
       </c>
-      <c r="G173" t="s">
+      <c r="H173" t="s">
         <v>1</v>
       </c>
       <c r="I173" t="s">
@@ -10315,7 +10318,7 @@
       <c r="E174" t="s">
         <v>41</v>
       </c>
-      <c r="G174" t="s">
+      <c r="H174" t="s">
         <v>1</v>
       </c>
       <c r="I174" t="s">
@@ -10357,7 +10360,7 @@
       <c r="E175" t="s">
         <v>41</v>
       </c>
-      <c r="G175" t="s">
+      <c r="H175" t="s">
         <v>1</v>
       </c>
       <c r="I175" t="s">
@@ -10399,7 +10402,7 @@
       <c r="E176" t="s">
         <v>41</v>
       </c>
-      <c r="G176" t="s">
+      <c r="H176" t="s">
         <v>1</v>
       </c>
       <c r="I176" t="s">
@@ -10441,7 +10444,7 @@
       <c r="E177" t="s">
         <v>41</v>
       </c>
-      <c r="G177" t="s">
+      <c r="H177" t="s">
         <v>1</v>
       </c>
       <c r="I177" t="s">
@@ -10483,7 +10486,7 @@
       <c r="E178" t="s">
         <v>41</v>
       </c>
-      <c r="G178" t="s">
+      <c r="H178" t="s">
         <v>1</v>
       </c>
       <c r="I178" t="s">
@@ -10525,7 +10528,7 @@
       <c r="E179" t="s">
         <v>41</v>
       </c>
-      <c r="G179" t="s">
+      <c r="H179" t="s">
         <v>1</v>
       </c>
       <c r="I179" t="s">
@@ -10567,7 +10570,7 @@
       <c r="E180" t="s">
         <v>41</v>
       </c>
-      <c r="G180" t="s">
+      <c r="H180" t="s">
         <v>1</v>
       </c>
       <c r="I180" t="s">
@@ -10609,7 +10612,7 @@
       <c r="E181" t="s">
         <v>41</v>
       </c>
-      <c r="G181" t="s">
+      <c r="H181" t="s">
         <v>1</v>
       </c>
       <c r="I181" t="s">
@@ -10651,7 +10654,7 @@
       <c r="E182" t="s">
         <v>41</v>
       </c>
-      <c r="G182" t="s">
+      <c r="H182" t="s">
         <v>1</v>
       </c>
       <c r="I182" t="s">
@@ -10693,7 +10696,7 @@
       <c r="E183" t="s">
         <v>41</v>
       </c>
-      <c r="G183" t="s">
+      <c r="H183" t="s">
         <v>1</v>
       </c>
       <c r="I183" t="s">
@@ -10735,7 +10738,7 @@
       <c r="E184" t="s">
         <v>41</v>
       </c>
-      <c r="G184" t="s">
+      <c r="H184" t="s">
         <v>1</v>
       </c>
       <c r="I184" t="s">
@@ -10777,7 +10780,7 @@
       <c r="E185" t="s">
         <v>41</v>
       </c>
-      <c r="G185" t="s">
+      <c r="H185" t="s">
         <v>1</v>
       </c>
       <c r="I185" t="s">
@@ -10819,7 +10822,7 @@
       <c r="E186" t="s">
         <v>41</v>
       </c>
-      <c r="G186" t="s">
+      <c r="H186" t="s">
         <v>1</v>
       </c>
       <c r="I186" t="s">
@@ -10861,7 +10864,7 @@
       <c r="E187" t="s">
         <v>41</v>
       </c>
-      <c r="G187" t="s">
+      <c r="H187" t="s">
         <v>1</v>
       </c>
       <c r="I187" t="s">
@@ -10903,7 +10906,7 @@
       <c r="E188" t="s">
         <v>41</v>
       </c>
-      <c r="G188" t="s">
+      <c r="H188" t="s">
         <v>1</v>
       </c>
       <c r="I188" t="s">
@@ -10945,7 +10948,7 @@
       <c r="E189" t="s">
         <v>41</v>
       </c>
-      <c r="G189" t="s">
+      <c r="H189" t="s">
         <v>1</v>
       </c>
       <c r="I189" t="s">
@@ -10987,7 +10990,7 @@
       <c r="E190" t="s">
         <v>41</v>
       </c>
-      <c r="G190" t="s">
+      <c r="H190" t="s">
         <v>1</v>
       </c>
       <c r="I190" t="s">
@@ -11029,7 +11032,7 @@
       <c r="E191" t="s">
         <v>41</v>
       </c>
-      <c r="G191" t="s">
+      <c r="H191" t="s">
         <v>1</v>
       </c>
       <c r="I191" t="s">
@@ -11071,7 +11074,7 @@
       <c r="E192" t="s">
         <v>41</v>
       </c>
-      <c r="G192" t="s">
+      <c r="H192" t="s">
         <v>1</v>
       </c>
       <c r="I192" t="s">
@@ -11113,7 +11116,7 @@
       <c r="E193" t="s">
         <v>41</v>
       </c>
-      <c r="G193" t="s">
+      <c r="H193" t="s">
         <v>1</v>
       </c>
       <c r="I193" t="s">
@@ -11155,7 +11158,7 @@
       <c r="E194" t="s">
         <v>42</v>
       </c>
-      <c r="G194" t="s">
+      <c r="H194" t="s">
         <v>43</v>
       </c>
       <c r="I194" t="s">
@@ -11197,7 +11200,7 @@
       <c r="E195" t="s">
         <v>42</v>
       </c>
-      <c r="G195" t="s">
+      <c r="H195" t="s">
         <v>43</v>
       </c>
       <c r="I195" t="s">
@@ -11239,7 +11242,7 @@
       <c r="E196" t="s">
         <v>42</v>
       </c>
-      <c r="G196" t="s">
+      <c r="H196" t="s">
         <v>43</v>
       </c>
       <c r="I196" t="s">
@@ -11281,7 +11284,7 @@
       <c r="E197" t="s">
         <v>42</v>
       </c>
-      <c r="G197" t="s">
+      <c r="H197" t="s">
         <v>43</v>
       </c>
       <c r="I197" t="s">

</xml_diff>